<commit_message>
Ajout mcd & mpd
</commit_message>
<xml_diff>
--- a/Livrables/MCD et MPD mediastore v2.xlsx
+++ b/Livrables/MCD et MPD mediastore v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="23715" windowHeight="8775" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="23715" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="MCD" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="146">
   <si>
     <t>nom</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>date commande</t>
-  </si>
-  <si>
-    <t>statut</t>
   </si>
   <si>
     <t>0,n</t>
@@ -457,6 +454,12 @@
   </si>
   <si>
     <t>Avancement GLOBAL</t>
+  </si>
+  <si>
+    <t>seuil</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -1134,13 +1137,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1184,20 +1187,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>639536</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>80296</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>29935</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPr id="2" name="Image 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1216,8 +1219,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9783536" cy="9795796"/>
+          <a:off x="775607" y="217714"/>
+          <a:ext cx="9178018" cy="8384721"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1516,9 +1519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:K42"/>
+  <dimension ref="C2:K44"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1531,13 +1536,13 @@
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
@@ -1567,28 +1572,28 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>1.1000000000000001</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
       <c r="I5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J5">
         <v>1.1000000000000001</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">
@@ -1628,18 +1633,18 @@
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G13" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
@@ -1650,52 +1655,52 @@
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G15" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.25">
       <c r="K16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.25">
       <c r="K17" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="7:11" x14ac:dyDescent="0.25">
       <c r="K18" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="7:11" x14ac:dyDescent="0.25">
       <c r="K19" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="7:11" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G21" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G23" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K23" s="11"/>
     </row>
@@ -1707,69 +1712,73 @@
     </row>
     <row r="25" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K25" s="11"/>
     </row>
     <row r="26" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K26" s="11"/>
     </row>
     <row r="27" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G29" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G30" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G31" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G32" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G30" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G31" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G34" s="27" t="s">
+      <c r="G33" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G35" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G36" s="1" t="s">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="1"/>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G39" s="1"/>
@@ -1781,7 +1790,13 @@
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G42" s="2"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G44" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1793,7 +1808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
@@ -1818,297 +1833,297 @@
   <sheetData>
     <row r="2" spans="2:4" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="55"/>
       <c r="D2" s="56"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2148,7 +2163,7 @@
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D2" s="58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" s="59"/>
       <c r="F2" s="59"/>
@@ -2204,19 +2219,19 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -2263,7 +2278,7 @@
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="C6" s="45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -2288,13 +2303,13 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -2305,7 +2320,7 @@
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
@@ -2321,13 +2336,13 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -2338,7 +2353,7 @@
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
@@ -2354,13 +2369,13 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -2372,7 +2387,7 @@
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
       <c r="M9" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
@@ -2387,13 +2402,13 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -2418,13 +2433,13 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="14"/>
@@ -2435,7 +2450,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
@@ -2451,13 +2466,13 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -2468,7 +2483,7 @@
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
@@ -2511,7 +2526,7 @@
       <c r="A14" s="28"/>
       <c r="B14" s="22"/>
       <c r="C14" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -2536,13 +2551,13 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -2554,7 +2569,7 @@
       <c r="K15" s="10"/>
       <c r="L15" s="21"/>
       <c r="M15" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -2569,13 +2584,13 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -2600,13 +2615,13 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="16"/>
@@ -2618,7 +2633,7 @@
       <c r="K17" s="16"/>
       <c r="L17" s="20"/>
       <c r="M17" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2633,13 +2648,13 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
@@ -2651,7 +2666,7 @@
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
@@ -2666,13 +2681,13 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -2684,7 +2699,7 @@
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
       <c r="M19" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
@@ -2731,16 +2746,16 @@
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="35">
         <v>1</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -2752,93 +2767,93 @@
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="22"/>
       <c r="C4" s="45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" s="39"/>
       <c r="E4" s="40"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" s="37">
         <v>1</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="37">
         <v>1</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D7" s="37">
         <v>1</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" s="37">
         <v>0.5</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" s="37">
         <v>1</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D10" s="37">
         <v>0.75</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -2850,84 +2865,84 @@
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
       <c r="C12" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D12" s="41"/>
       <c r="E12" s="42"/>
     </row>
     <row r="13" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D13" s="37">
         <v>0.25</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14" s="37">
         <v>0.75</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" s="37">
         <v>0.5</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16" s="37">
         <v>0.5</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" s="43">
         <v>0.5</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C18" s="52" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D18" s="53">
         <f>SUM(D2:D17)/12</f>

</xml_diff>

<commit_message>
MàJ doc par JB
</commit_message>
<xml_diff>
--- a/Livrables/MCD et MPD mediastore v2.xlsx
+++ b/Livrables/MCD et MPD mediastore v2.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="144">
   <si>
     <t>nom</t>
   </si>
@@ -308,9 +308,6 @@
     <t>p4</t>
   </si>
   <si>
-    <t>En Cours</t>
-  </si>
-  <si>
     <t>Terminé</t>
   </si>
   <si>
@@ -348,9 +345,6 @@
   </si>
   <si>
     <t>11.6 : intégration au site</t>
-  </si>
-  <si>
-    <t>En cours</t>
   </si>
   <si>
     <t>All</t>
@@ -1521,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,7 +1575,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -1742,12 +1736,12 @@
     </row>
     <row r="30" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G30" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G31" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="7:11" x14ac:dyDescent="0.25">
@@ -1767,12 +1761,12 @@
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G36" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G37" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.25">
@@ -1800,7 +1794,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1843,7 +1838,7 @@
         <v>43</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -1888,10 +1883,10 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -1936,10 +1931,10 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -1984,10 +1979,10 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -2032,7 +2027,7 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>85</v>
@@ -2040,7 +2035,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D41" t="s">
         <v>59</v>
@@ -2048,7 +2043,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D42" t="s">
         <v>60</v>
@@ -2056,7 +2051,7 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
         <v>61</v>
@@ -2064,7 +2059,7 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D44" t="s">
         <v>62</v>
@@ -2072,7 +2067,7 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D45" t="s">
         <v>63</v>
@@ -2080,7 +2075,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>42</v>
@@ -2088,7 +2083,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
         <v>64</v>
@@ -2096,7 +2091,7 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D51" t="s">
         <v>65</v>
@@ -2104,7 +2099,7 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D52" t="s">
         <v>66</v>
@@ -2112,7 +2107,7 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D53" t="s">
         <v>67</v>
@@ -2120,7 +2115,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D54" t="s">
         <v>68</v>
@@ -2142,23 +2137,28 @@
   </sheetPr>
   <dimension ref="A2:W19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="5.5703125" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="5.5703125" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.5703125" customWidth="1"/>
-    <col min="12" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.5703125" customWidth="1"/>
     <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="23" width="5.5703125" customWidth="1"/>
+    <col min="16" max="18" width="5.5703125" customWidth="1"/>
+    <col min="19" max="19" width="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -2219,19 +2219,19 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -2278,7 +2278,7 @@
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="C6" s="45" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -2309,7 +2309,7 @@
         <v>87</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -2320,7 +2320,7 @@
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
@@ -2342,7 +2342,7 @@
         <v>87</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -2353,7 +2353,7 @@
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
@@ -2375,7 +2375,7 @@
         <v>86</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -2386,15 +2386,15 @@
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
-      <c r="M9" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16" t="s">
+        <v>113</v>
+      </c>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
@@ -2408,7 +2408,7 @@
         <v>86</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -2439,7 +2439,7 @@
         <v>87</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="14"/>
@@ -2450,7 +2450,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
@@ -2472,7 +2472,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -2482,17 +2482,17 @@
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
-      <c r="L12" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
@@ -2526,7 +2526,7 @@
       <c r="A14" s="28"/>
       <c r="B14" s="22"/>
       <c r="C14" s="46" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -2557,7 +2557,7 @@
         <v>88</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -2568,15 +2568,15 @@
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="21"/>
-      <c r="M15" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
@@ -2590,7 +2590,7 @@
         <v>86</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -2621,7 +2621,7 @@
         <v>86</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="16"/>
@@ -2632,16 +2632,16 @@
       <c r="J17" s="20"/>
       <c r="K17" s="16"/>
       <c r="L17" s="20"/>
-      <c r="M17" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16" t="s">
+        <v>113</v>
+      </c>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
@@ -2654,7 +2654,7 @@
         <v>88</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
@@ -2665,29 +2665,29 @@
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
-      <c r="M18" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21" t="s">
+        <v>113</v>
+      </c>
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -2698,17 +2698,17 @@
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
-      <c r="M19" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="18" t="s">
+        <v>113</v>
+      </c>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
     </row>
@@ -2731,7 +2731,7 @@
   <dimension ref="B1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,16 +2746,16 @@
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="35">
         <v>1</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -2767,7 +2767,7 @@
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="22"/>
       <c r="C4" s="45" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D4" s="39"/>
       <c r="E4" s="40"/>
@@ -2777,13 +2777,13 @@
         <v>87</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D5" s="37">
         <v>1</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -2791,13 +2791,13 @@
         <v>87</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D6" s="37">
         <v>1</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -2805,13 +2805,13 @@
         <v>86</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D7" s="37">
         <v>1</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -2819,13 +2819,13 @@
         <v>86</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D8" s="37">
         <v>0.5</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -2833,13 +2833,13 @@
         <v>87</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D9" s="37">
         <v>1</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -2847,13 +2847,13 @@
         <v>88</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D10" s="37">
         <v>0.75</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -2865,7 +2865,7 @@
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
       <c r="C12" s="46" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D12" s="41"/>
       <c r="E12" s="42"/>
@@ -2875,13 +2875,13 @@
         <v>88</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D13" s="37">
         <v>0.25</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -2889,13 +2889,13 @@
         <v>86</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D14" s="37">
         <v>0.75</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -2903,13 +2903,13 @@
         <v>86</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D15" s="37">
         <v>0.5</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -2917,32 +2917,32 @@
         <v>88</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D16" s="37">
         <v>0.5</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D17" s="43">
         <v>0.5</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C18" s="52" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D18" s="53">
         <f>SUM(D2:D17)/12</f>

</xml_diff>

<commit_message>
MàJ doc JB the last?
</commit_message>
<xml_diff>
--- a/Livrables/MCD et MPD mediastore v2.xlsx
+++ b/Livrables/MCD et MPD mediastore v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="23715" windowHeight="8775"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="23715" windowHeight="8775" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MCD" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="144">
   <si>
     <t>nom</t>
   </si>
@@ -1515,7 +1515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:K44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
@@ -2137,8 +2137,8 @@
   </sheetPr>
   <dimension ref="A2:W19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2540,10 +2540,12 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49" t="s">
+        <v>113</v>
+      </c>
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
@@ -2605,9 +2607,11 @@
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49" t="s">
+        <v>113</v>
+      </c>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>

</xml_diff>